<commit_message>
Update descriptions by incorporating comments from reviewers.
	modified:   RMLands Landcover Type Descriptions FAQ.docx
	modified:   _CMM/Curlleaf Mountain Mahogany Draft Description.docx
	modified:   _DFTO/Doug Fir Tanoak Draft Description.docx
	modified:   _LPN/LPN Draft Description.docx
	modified:   _LSG/Black and Low Sagebrush Draft Description.docx
	modified:   _MHW/Montane Hardwood Draft Description.docx
	modified:   _MRIP/Montane Riparian Draft Description.docx
	modified:   _OCFW/OCFW Class Transitions.xlsx
	modified:   _RFR/RFR Draft Description.docx
	modified:   _SAGE/Big Sagebrush Draft Description.docx
	modified:   _SCN/Subalpine Conifer Draft Description.docx
</commit_message>
<xml_diff>
--- a/_OCFW/OCFW Class Transitions.xlsx
+++ b/_OCFW/OCFW Class Transitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="23620" windowWidth="12980" windowHeight="15920" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="31440" windowHeight="23560" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OCFW" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="ASP4" sheetId="14" r:id="rId3"/>
     <sheet name="OCFW 4-class" sheetId="15" r:id="rId4"/>
     <sheet name="UM 4-class" sheetId="16" r:id="rId5"/>
+    <sheet name="test" sheetId="17" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="59">
   <si>
     <t>Succession Type</t>
   </si>
@@ -318,8 +319,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -443,7 +448,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -493,6 +498,8 @@
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -542,6 +549,8 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2236,7 +2245,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" ref="C9:G10" si="1">1/D3</f>
+        <f t="shared" ref="D10:F10" si="1">1/D3</f>
         <v>6.6666666666666671E-3</v>
       </c>
       <c r="E10" s="7">
@@ -2612,7 +2621,7 @@
         <v>0.18330844810123939</v>
       </c>
       <c r="E31" s="21">
-        <f t="shared" ref="D31:G31" si="10">E17/$H$17</f>
+        <f t="shared" ref="E31:G31" si="10">E17/$H$17</f>
         <v>0.21671034633978262</v>
       </c>
       <c r="F31" s="21">
@@ -5858,8 +5867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7082,8 +7091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7611,7 +7620,7 @@
         <v>0.22913615824960651</v>
       </c>
       <c r="E31" s="21">
-        <f t="shared" ref="E31:H31" si="9">E17/$H$17</f>
+        <f t="shared" ref="E31:G31" si="9">E17/$H$17</f>
         <v>0.27088864003591834</v>
       </c>
       <c r="F31" s="21">
@@ -8185,6 +8194,1202 @@
       <c r="I63">
         <f>1/H63</f>
         <v>9.4442266798381613</v>
+      </c>
+      <c r="J63">
+        <f>J58+J62</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6">
+        <v>175</v>
+      </c>
+      <c r="D2" s="6">
+        <v>250</v>
+      </c>
+      <c r="E2" s="6">
+        <v>160</v>
+      </c>
+      <c r="F2" s="6">
+        <v>250</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>75</v>
+      </c>
+      <c r="D3" s="6">
+        <v>150</v>
+      </c>
+      <c r="E3" s="6">
+        <v>66</v>
+      </c>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6">
+        <v>20</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7">
+        <f>1/C2</f>
+        <v>5.7142857142857143E-3</v>
+      </c>
+      <c r="D9" s="7">
+        <f>1/D2</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" ref="D9:F10" si="0">1/E2</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7">
+        <f>1/C3</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7">
+        <f>C10</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" ref="D12:F12" si="1">D10</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <f>1/C6</f>
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" ref="D13:F13" si="2">1/D6</f>
+        <v>0.05</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="7">
+        <f>C9+C11+C13</f>
+        <v>6.9047619047619052E-2</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" ref="D14:F14" si="3">D9+D11</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="3"/>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7">
+        <f>SUM(C14:G14)</f>
+        <v>8.3297619047619065E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7">
+        <f t="shared" ref="D15:F15" si="4">D12+D13</f>
+        <v>5.6666666666666671E-2</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="4"/>
+        <v>6.5151515151515155E-2</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="4"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7">
+        <f>SUM(C15:G15)</f>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7">
+        <f>C9+C10+C13</f>
+        <v>6.9047619047619052E-2</v>
+      </c>
+      <c r="D17" s="7">
+        <f>D9+D10+D13</f>
+        <v>6.0666666666666674E-2</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" ref="D17:F17" si="5">E9+E10+E13</f>
+        <v>7.140151515151516E-2</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="5"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7">
+        <f>SUM(C17:G17)</f>
+        <v>0.26511580086580089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="7">
+        <f>C14+C15</f>
+        <v>6.9047619047619052E-2</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" ref="D18:F18" si="6">D14+D15</f>
+        <v>6.0666666666666674E-2</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="6"/>
+        <v>7.140151515151516E-2</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" si="6"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <f>G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7" t="e">
+        <f>1/G6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7">
+        <f t="shared" ref="E26" si="7">SUM(E21:E23)</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="7">
+        <f>SUM(F21:F25)</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="e">
+        <f>SUM(G21:G25)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <f>C11/C14</f>
+        <v>0.19310344827586207</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28:G29" si="8">E11/E14</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G28" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="8"/>
+        <v>0.23255813953488372</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="8"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G29" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="C30">
+        <v>0.2092</v>
+      </c>
+      <c r="D30">
+        <v>0.18060000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.21360000000000001</v>
+      </c>
+      <c r="F30">
+        <v>0.2064</v>
+      </c>
+      <c r="G30">
+        <v>0.19020000000000001</v>
+      </c>
+      <c r="H30">
+        <f>SUM(C30:G30)</f>
+        <v>1</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21">
+        <f>C17/$H$17</f>
+        <v>0.26044324337563834</v>
+      </c>
+      <c r="D31" s="21">
+        <f>D17/$H$17</f>
+        <v>0.2288308221107333</v>
+      </c>
+      <c r="E31" s="21">
+        <f t="shared" ref="E31:G31" si="9">E17/$H$17</f>
+        <v>0.26932199030889875</v>
+      </c>
+      <c r="F31" s="21">
+        <f t="shared" si="9"/>
+        <v>0.2414039442047296</v>
+      </c>
+      <c r="G31" s="21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f>SUM(C31:G31)</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21">
+        <f>C14/C17</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="21">
+        <f t="shared" ref="D32:F32" si="10">D14/D17</f>
+        <v>6.5934065934065922E-2</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="10"/>
+        <v>8.7533156498673728E-2</v>
+      </c>
+      <c r="F32" s="21">
+        <f t="shared" si="10"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G32" s="21" t="e">
+        <f>G14/G17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32">
+        <f>H14/$H$14</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21">
+        <f>C15/C17</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="21">
+        <f t="shared" ref="D33:G33" si="11">D15/D17</f>
+        <v>0.93406593406593397</v>
+      </c>
+      <c r="E33" s="21">
+        <f t="shared" si="11"/>
+        <v>0.91246684350132623</v>
+      </c>
+      <c r="F33" s="21">
+        <f t="shared" si="11"/>
+        <v>0.9375</v>
+      </c>
+      <c r="G33" s="21" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33">
+        <f>H15/$H$15</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <f>C32</f>
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <f>E32</f>
+        <v>8.7533156498673728E-2</v>
+      </c>
+      <c r="F36">
+        <f>F32</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G36" t="e">
+        <f>G32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <f>E33</f>
+        <v>0.91246684350132623</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>F33</f>
+        <v>0.9375</v>
+      </c>
+      <c r="G39" t="e">
+        <f>(1/G3)/G17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="e">
+        <f>(G13)/G17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <f>SUM(C36:C40)</f>
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ref="E41:F41" si="12">SUM(E36:E40)</f>
+        <v>1</v>
+      </c>
+      <c r="F41" s="9">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="G41" t="e">
+        <f>SUM(G36:G40)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="7">
+        <f>E38/E33</f>
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <f>F39/F33</f>
+        <v>1</v>
+      </c>
+      <c r="G46" t="e">
+        <f>G39/G33</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" t="e">
+        <f>G40/G33</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48">
+        <f>SUM(C44:C47)</f>
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48:G48" si="13">SUM(E44:E47)</f>
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G48" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50">
+        <v>0.15</v>
+      </c>
+      <c r="D50">
+        <v>0.05</v>
+      </c>
+      <c r="E50">
+        <v>0.25</v>
+      </c>
+      <c r="F50">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H50">
+        <f>SUM(C50:G50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52">
+        <f>C17*C50</f>
+        <v>1.0357142857142858E-2</v>
+      </c>
+      <c r="D52">
+        <f>D17*D50</f>
+        <v>3.0333333333333341E-3</v>
+      </c>
+      <c r="E52">
+        <f>E17*E50</f>
+        <v>1.785037878787879E-2</v>
+      </c>
+      <c r="F52">
+        <f>F17*F50</f>
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="G52">
+        <f>G17*G50</f>
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <f>SUM(C52:G52)</f>
+        <v>6.6440854978354988E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53">
+        <f>C14*C50</f>
+        <v>1.0357142857142858E-2</v>
+      </c>
+      <c r="D53">
+        <f>D14*D50</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E53">
+        <f>E14*E50</f>
+        <v>1.5625000000000001E-3</v>
+      </c>
+      <c r="F53">
+        <f>F14*F50</f>
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="G53">
+        <f>G14*G50</f>
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <f>SUM(C53:G53)</f>
+        <v>1.4319642857142859E-2</v>
+      </c>
+      <c r="J53">
+        <f>0.2*0.02+0.1*1/75+0.25*1/315+0.4*0.001+0.05*1/60</f>
+        <v>7.3603174603174611E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54">
+        <f>C15*C50</f>
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <f>D15*D50</f>
+        <v>2.8333333333333335E-3</v>
+      </c>
+      <c r="E54">
+        <f>E15*E50</f>
+        <v>1.6287878787878789E-2</v>
+      </c>
+      <c r="F54">
+        <f>F15*F50</f>
+        <v>3.3000000000000008E-2</v>
+      </c>
+      <c r="G54">
+        <f>G15*G50</f>
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <f>SUM(C54:G54)</f>
+        <v>5.2121212121212131E-2</v>
+      </c>
+      <c r="J54">
+        <f>H14/H17</f>
+        <v>0.3141933403274727</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" t="s">
+        <v>41</v>
+      </c>
+      <c r="H57" t="s">
+        <v>42</v>
+      </c>
+      <c r="I57" t="s">
+        <v>38</v>
+      </c>
+      <c r="J57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="7">
+        <f>1/C58</f>
+        <v>149.92503748125938</v>
+      </c>
+      <c r="C58">
+        <v>6.6699999999999997E-3</v>
+      </c>
+      <c r="D58">
+        <f>C58/C63</f>
+        <v>0.11608075182735816</v>
+      </c>
+      <c r="F58">
+        <f>F63*D58</f>
+        <v>7.7125043979399191E-3</v>
+      </c>
+      <c r="H58">
+        <f>H53</f>
+        <v>1.4319642857142859E-2</v>
+      </c>
+      <c r="I58">
+        <f>1/H58</f>
+        <v>69.834143908217968</v>
+      </c>
+      <c r="J58">
+        <f>H58/H63</f>
+        <v>0.2155246626764194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="7">
+        <f t="shared" ref="B59:B63" si="14">1/C59</f>
+        <v>45.004500450045008</v>
+      </c>
+      <c r="C59">
+        <v>2.222E-2</v>
+      </c>
+      <c r="D59">
+        <f>C59/C63</f>
+        <v>0.38670379394361298</v>
+      </c>
+      <c r="F59">
+        <f>F63*D59</f>
+        <v>2.5692930692987261E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="7">
+        <f t="shared" si="14"/>
+        <v>35.001750087504377</v>
+      </c>
+      <c r="C62">
+        <v>2.8570000000000002E-2</v>
+      </c>
+      <c r="D62">
+        <f>C62/C63</f>
+        <v>0.49721545422902896</v>
+      </c>
+      <c r="F62">
+        <f>F63*D62</f>
+        <v>3.3035419887427815E-2</v>
+      </c>
+      <c r="H62">
+        <f>H54</f>
+        <v>5.2121212121212131E-2</v>
+      </c>
+      <c r="I62">
+        <f>1/H62</f>
+        <v>19.186046511627904</v>
+      </c>
+      <c r="J62">
+        <f>H62/H63</f>
+        <v>0.78447533732358066</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="7">
+        <f t="shared" si="14"/>
+        <v>17.40341106856944</v>
+      </c>
+      <c r="C63">
+        <v>5.7459999999999997E-2</v>
+      </c>
+      <c r="D63">
+        <f>D58+D59+D62</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="F63">
+        <f>H52</f>
+        <v>6.6440854978354988E-2</v>
+      </c>
+      <c r="H63">
+        <f>H58+H62</f>
+        <v>6.6440854978354988E-2</v>
+      </c>
+      <c r="I63">
+        <f>1/H63</f>
+        <v>15.050980309115207</v>
       </c>
       <c r="J63">
         <f>J58+J62</f>

</xml_diff>